<commit_message>
V3 Basic full Roadmap
</commit_message>
<xml_diff>
--- a/PRM-Data.xlsx
+++ b/PRM-Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Product-Roadmapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2929A24-F011-4ED5-9106-D056F2B69EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34A1C51-A3B1-48D4-8F41-638048EA8AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-14205" windowWidth="16440" windowHeight="28320" xr2:uid="{C670BAD3-E4C4-4E4C-99CD-E2A94FFBDAC2}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{C670BAD3-E4C4-4E4C-99CD-E2A94FFBDAC2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Technology" sheetId="1" r:id="rId1"/>
-    <sheet name="Capabilities" sheetId="2" r:id="rId2"/>
+    <sheet name="Roadmap" sheetId="3" r:id="rId1"/>
+    <sheet name="Technology" sheetId="1" r:id="rId2"/>
+    <sheet name="Capabilities" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
   <si>
     <t>Start Date</t>
   </si>
@@ -112,6 +113,111 @@
   </si>
   <si>
     <t>T02, T03</t>
+  </si>
+  <si>
+    <t>Timeline Risk</t>
+  </si>
+  <si>
+    <t>Exp. Budget</t>
+  </si>
+  <si>
+    <t>Budget Risk</t>
+  </si>
+  <si>
+    <t>Risk Rating</t>
+  </si>
+  <si>
+    <t>Product line ID</t>
+  </si>
+  <si>
+    <t>Track ID</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>Feasibility Study</t>
+  </si>
+  <si>
+    <t>PL1</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>Concept Development</t>
+  </si>
+  <si>
+    <t>Product Architecture</t>
+  </si>
+  <si>
+    <t>Prototype Build</t>
+  </si>
+  <si>
+    <t>#d62728</t>
+  </si>
+  <si>
+    <t>Field Testing</t>
+  </si>
+  <si>
+    <t>#9467bd</t>
+  </si>
+  <si>
+    <t>Risk Review</t>
+  </si>
+  <si>
+    <t>#8c564b</t>
+  </si>
+  <si>
+    <t>Final Design Freeze</t>
+  </si>
+  <si>
+    <t>#e377c2</t>
+  </si>
+  <si>
+    <t>Manufacturing Setup</t>
+  </si>
+  <si>
+    <t>#7f7f7f</t>
+  </si>
+  <si>
+    <t>Low-Rate Production</t>
+  </si>
+  <si>
+    <t>#bcbd22</t>
+  </si>
+  <si>
+    <t>Market Launch Prep</t>
+  </si>
+  <si>
+    <t>#17becf</t>
   </si>
 </sst>
 </file>
@@ -167,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -182,6 +288,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,11 +628,454 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D41C1B-88B2-4367-9D4B-0EFA5AC22627}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="43.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.21875" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="8">
+        <v>45658</v>
+      </c>
+      <c r="D2" s="8">
+        <v>45717</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="H2" s="7">
+        <v>2</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="8">
+        <v>45703</v>
+      </c>
+      <c r="D3" s="8">
+        <v>45792</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="F3" s="7">
+        <v>2</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="H3" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="8">
+        <v>45778</v>
+      </c>
+      <c r="D4" s="8">
+        <v>45868</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="7">
+        <v>4.2</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="8">
+        <v>45870</v>
+      </c>
+      <c r="D5" s="8">
+        <v>45945</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="F5" s="7">
+        <v>5</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="H5" s="7">
+        <v>5</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="8">
+        <v>45950</v>
+      </c>
+      <c r="D6" s="8">
+        <v>46032</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="F6" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="H6" s="7">
+        <v>3.8</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="8">
+        <v>46037</v>
+      </c>
+      <c r="D7" s="8">
+        <v>46068</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="8">
+        <v>46073</v>
+      </c>
+      <c r="D8" s="8">
+        <v>46101</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="8">
+        <v>46113</v>
+      </c>
+      <c r="D9" s="8">
+        <v>46188</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F9" s="7">
+        <v>6</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
+        <v>5.5</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="8">
+        <v>46193</v>
+      </c>
+      <c r="D10" s="8">
+        <v>46285</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="F10" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="H10" s="7">
+        <v>6</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="8">
+        <v>46290</v>
+      </c>
+      <c r="D11" s="8">
+        <v>46341</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="7">
+        <v>3</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C67F632-76BE-4CDD-83AF-F7105F7A71A4}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,7 +1482,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149D8FBB-EAF5-4DE2-929F-DB10047ED436}">
   <dimension ref="A1:G5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Full Roadmap with milestones
</commit_message>
<xml_diff>
--- a/PRM-Data.xlsx
+++ b/PRM-Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Product-Roadmapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34A1C51-A3B1-48D4-8F41-638048EA8AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E56A0F-42DA-4772-8702-E8C667C23526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{C670BAD3-E4C4-4E4C-99CD-E2A94FFBDAC2}"/>
+    <workbookView xWindow="-16200" yWindow="-10710" windowWidth="16410" windowHeight="10005" activeTab="1" xr2:uid="{C670BAD3-E4C4-4E4C-99CD-E2A94FFBDAC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Roadmap" sheetId="3" r:id="rId1"/>
-    <sheet name="Technology" sheetId="1" r:id="rId2"/>
-    <sheet name="Capabilities" sheetId="2" r:id="rId3"/>
+    <sheet name="Milestones" sheetId="4" r:id="rId2"/>
+    <sheet name="Technology" sheetId="1" r:id="rId3"/>
+    <sheet name="Capabilities" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="81">
   <si>
     <t>Start Date</t>
   </si>
@@ -218,6 +219,69 @@
   </si>
   <si>
     <t>#17becf</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>MS01</t>
+  </si>
+  <si>
+    <t>Project Kickoff</t>
+  </si>
+  <si>
+    <t>MS02</t>
+  </si>
+  <si>
+    <t>Preliminary Design Review (PDR)</t>
+  </si>
+  <si>
+    <t>MS03</t>
+  </si>
+  <si>
+    <t>Critical Design Review (CDR)</t>
+  </si>
+  <si>
+    <t>MS04</t>
+  </si>
+  <si>
+    <t>First Prototype Assembled</t>
+  </si>
+  <si>
+    <t>MS05</t>
+  </si>
+  <si>
+    <t>First Integrated Demo</t>
+  </si>
+  <si>
+    <t>MS06</t>
+  </si>
+  <si>
+    <t>Software Feature Freeze</t>
+  </si>
+  <si>
+    <t>MS07</t>
+  </si>
+  <si>
+    <t>Final Demo / Customer Review</t>
+  </si>
+  <si>
+    <t>MS08</t>
+  </si>
+  <si>
+    <t>Production Decision Point</t>
+  </si>
+  <si>
+    <t>MS09</t>
+  </si>
+  <si>
+    <t>Initial Manufacturing Run</t>
+  </si>
+  <si>
+    <t>MS10</t>
+  </si>
+  <si>
+    <t>Product Launch</t>
   </si>
 </sst>
 </file>
@@ -631,7 +695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D41C1B-88B2-4367-9D4B-0EFA5AC22627}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -1071,6 +1135,185 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B143C62-0EA4-4B9F-9C66-E89626643288}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="8">
+        <v>45703</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="8">
+        <v>45748</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="8">
+        <v>45792</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="8">
+        <v>45848</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="8">
+        <v>45870</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="8">
+        <v>45915</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="8">
+        <v>45945</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="8">
+        <v>45962</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="8">
+        <v>46037</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="8">
+        <v>46082</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F12" s="8"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F13" s="8"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F14" s="8"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F15" s="8"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C67F632-76BE-4CDD-83AF-F7105F7A71A4}">
   <dimension ref="A1:G48"/>
   <sheetViews>
@@ -1482,7 +1725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149D8FBB-EAF5-4DE2-929F-DB10047ED436}">
   <dimension ref="A1:G5"/>
   <sheetViews>

</xml_diff>